<commit_message>
Added visualization on tweet sentiments
</commit_message>
<xml_diff>
--- a/dataset/tweet-sample-100.xlsx
+++ b/dataset/tweet-sample-100.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\cancelled\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE98A41C-3447-4224-80A6-2EF55BFA8608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{810543DD-C915-48F8-8E5A-8CE6A33C331F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5B3E8B93-712B-46CE-8E6F-A7339A9A22EE}"/>
   </bookViews>
@@ -772,11 +772,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81BFBB02-04D4-4B0D-8ADF-6CE82F663A63}">
   <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B100"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="A93" sqref="A93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="180.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>